<commit_message>
Doku: Archivische Ablieferungsschnittstelle Stand 2014-10-01
</commit_message>
<xml_diff>
--- a/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
+++ b/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\eCH\Fachgruppe_Digitale_Archivierung\eCH-0160 Archivische Ablieferungsschnittstelle (SIP)\v1.1\03_Dokumentation\2_Entwurf_v1.1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Titelblatt" sheetId="1" r:id="rId1"/>
@@ -14,45 +19,55 @@
     <sheet name="Ordnungssystem" sheetId="5" r:id="rId5"/>
     <sheet name="Ordnungssystemposition" sheetId="6" r:id="rId6"/>
     <sheet name="Dossier" sheetId="7" r:id="rId7"/>
-    <sheet name="Dokument" sheetId="8" r:id="rId8"/>
-    <sheet name="Ordner" sheetId="9" r:id="rId9"/>
-    <sheet name="Datei" sheetId="10" r:id="rId10"/>
-    <sheet name="Arch. Vorgang" sheetId="11" r:id="rId11"/>
-    <sheet name="Dokumentation" sheetId="12" r:id="rId12"/>
+    <sheet name="Vorgang" sheetId="14" r:id="rId8"/>
+    <sheet name="Aktivität" sheetId="13" r:id="rId9"/>
+    <sheet name="Dokument" sheetId="8" r:id="rId10"/>
+    <sheet name="Ordner" sheetId="9" r:id="rId11"/>
+    <sheet name="Datei" sheetId="10" r:id="rId12"/>
+    <sheet name="Arch. Vorgang" sheetId="11" r:id="rId13"/>
+    <sheet name="Dokumentation" sheetId="12" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_Toc241581282" localSheetId="11">Dokumentation!$A$25</definedName>
-    <definedName name="_Toc241581283" localSheetId="11">Dokumentation!$A$32</definedName>
+    <definedName name="_Toc241581282" localSheetId="13">Dokumentation!$A$25</definedName>
+    <definedName name="_Toc241581283" localSheetId="13">Dokumentation!$A$32</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Ablieferung!$A$1:$K$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">Dokument!$A$1:$K$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="8">Aktivität!$A$1:$K$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="9">Dokument!$A$1:$K$19</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Dossier!$A$1:$K$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">Ordnungssystem!$A$1:$K$9</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">Ordnungssystemposition!$A$1:$K$16</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Provenienz!$A$1:$K$12</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">Vorgang!$A$1:$K$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Ablieferung!$3:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="9">Datei!$3:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="7">Dokument!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="8">Aktivität!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="11">Datei!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="9">Dokument!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="6">Dossier!$3:$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="8">Ordner!$3:$3</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="10">Ordner!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="4">Ordnungssystem!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="5">Ordnungssystemposition!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">Provenienz!$3:$3</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Titelblatt!$A:$A,Titelblatt!$4:$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="7">Vorgang!$3:$3</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="2" hidden="1">Ablieferung!$A$1:$K$14</definedName>
-    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="7" hidden="1">Dokument!$A$1:$K$18</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="8" hidden="1">Aktivität!$A$1:$K$4</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="9" hidden="1">Dokument!$A$1:$K$18</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="6" hidden="1">Dossier!$A$1:$K$27</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="4" hidden="1">Ordnungssystem!$A$1:$K$8</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="5" hidden="1">Ordnungssystemposition!$A$1:$K$15</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="3" hidden="1">Provenienz!$A$1:$K$12</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintArea" localSheetId="7" hidden="1">Vorgang!$A$1:$K$4</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="2" hidden="1">Ablieferung!$3:$3</definedName>
-    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="9" hidden="1">Datei!$3:$3</definedName>
-    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="7" hidden="1">Dokument!$3:$3</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="8" hidden="1">Aktivität!$3:$3</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="11" hidden="1">Datei!$3:$3</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="9" hidden="1">Dokument!$3:$3</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="6" hidden="1">Dossier!$3:$3</definedName>
-    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="8" hidden="1">Ordner!$3:$3</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="10" hidden="1">Ordner!$3:$3</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="4" hidden="1">Ordnungssystem!$3:$3</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="5" hidden="1">Ordnungssystemposition!$3:$3</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="3" hidden="1">Provenienz!$3:$3</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="0" hidden="1">Titelblatt!$A:$A,Titelblatt!$4:$5</definedName>
+    <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="7" hidden="1">Vorgang!$3:$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <customWorkbookViews>
@@ -62,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="426">
   <si>
     <t xml:space="preserve">Systeme, die mit dem beschriebenen System Daten ausgetauscht haben und damit Subsysteme, Parallelsysteme oder übergeordnete Systeme sind. Hier werden die Bezeichnungen der Systeme und die Art der Verwandtschaft eingetragen. </t>
   </si>
@@ -945,9 +960,6 @@
   </si>
   <si>
     <t>Entstehungszeitraum Anmerkung</t>
-  </si>
-  <si>
-    <t>Vorgang</t>
   </si>
   <si>
     <t>Datei Referenz</t>
@@ -1475,12 +1487,139 @@
  * ca.01.02.2007-ca.01.05.2007</t>
     </r>
   </si>
+  <si>
+    <t>Entität: Vorgang</t>
+  </si>
+  <si>
+    <t>Arbeitsanweisung</t>
+  </si>
+  <si>
+    <t>arbeitsanweisung</t>
+  </si>
+  <si>
+    <t>Verweis</t>
+  </si>
+  <si>
+    <t>verweis</t>
+  </si>
+  <si>
+    <t>Benennung von Tätigkeit und Gegenstand des Geschäftsvorfalles.</t>
+  </si>
+  <si>
+    <t>Arbeitsanweisung, bzw.Auftragsbeschreibung: Vorgaben und Hinweise für die Durchführung und Erledigung.</t>
+  </si>
+  <si>
+    <t>Referenz auf andere Ordnungssystempositionen, Dossiers oder Vorgänge, die in enger Beziehung mit dem Vorgang stehen ohne direkt mit ihm verknüpft zu sein.</t>
+  </si>
+  <si>
+    <t>Polio-Impfaktion Herbst 1975</t>
+  </si>
+  <si>
+    <t>Impfplan und Zusammenstellen der Impfkosten für die Polio-Schutzimpfung 1975</t>
+  </si>
+  <si>
+    <t>Schirmbild und obligatorischen Tuberkulose-untersuchung</t>
+  </si>
+  <si>
+    <t>Entität: Aktivität</t>
+  </si>
+  <si>
+    <t>Vorschreibung</t>
+  </si>
+  <si>
+    <t>vorschreibung</t>
+  </si>
+  <si>
+    <t>akteur</t>
+  </si>
+  <si>
+    <t>Akteur</t>
+  </si>
+  <si>
+    <t>abschlussvermerk</t>
+  </si>
+  <si>
+    <t>Abschlussvermerk</t>
+  </si>
+  <si>
+    <t>Beschreibung der Tätigkeit, die ausgeführt werden soll.</t>
+  </si>
+  <si>
+    <t>Akteur, welcher die Aktivität durchführt. Im Organigramm bzw. den Organisationsvorschriften der Verwaltungseinheit aufgeführte Rollen bzw. Personen.</t>
+  </si>
+  <si>
+    <t>Kurze Beschreibung des Ergebnisses der Aktivität.</t>
+  </si>
+  <si>
+    <t>Tag, an dem die Aktivität abgeschlossen worden ist.</t>
+  </si>
+  <si>
+    <t>Referenz auf andere Ordnungssystempositionen, Dossiers, Vorgänge oder Aktivitäten, die in enger Beziehung zu der Aktivität stehen ohne direkt mit ihr verknüpft zu sein.</t>
+  </si>
+  <si>
+    <t>Informationen, die für die Aktivität von Bedeutung sind.</t>
+  </si>
+  <si>
+    <t>Heinz Mustermann</t>
+  </si>
+  <si>
+    <t>Dossier anlegen</t>
+  </si>
+  <si>
+    <t>Alle notwendigen Dokumente angelegt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(*)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Aus Gründen der Rückwärtskompatibilität mit Version 1.0 kann Vorgang auch weiterhin als Attribut der Entität Dossier verwendet werden.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Vorgang</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (*)</t>
+    </r>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>order</t>
+  </si>
+  <si>
+    <t>Ordnungszahl welche die Reihenfolge von Vorgängen innerhalb eines Dossiers festlegt, muss innerhalb des selben Dossier eindeutig sein.</t>
+  </si>
+  <si>
+    <t>Ordnungszahl welche die Reihenfolge von Aktivitäten innerhalb eines Dossiers festlegt, muss innerhalb des selben Vorgangs eindeutig sein.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1605,6 +1744,19 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1880,7 +2032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2128,26 +2280,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2158,16 +2298,31 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2247,6 +2402,14 @@
       <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3151,9 +3314,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3191,9 +3354,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3225,9 +3388,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3259,9 +3423,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3434,17 +3599,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="36" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" style="41"/>
@@ -3452,20 +3617,20 @@
     <col min="4" max="16384" width="11.42578125" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="36" customFormat="1" ht="99" customHeight="1">
+    <row r="1" spans="1:13" s="36" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M1"/>
     </row>
-    <row r="2" spans="1:13" s="39" customFormat="1" ht="63" customHeight="1">
+    <row r="2" spans="1:13" s="39" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="37"/>
       <c r="B2" s="38"/>
     </row>
-    <row r="3" spans="1:13" s="39" customFormat="1" ht="63" customHeight="1">
+    <row r="3" spans="1:13" s="39" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="37"/>
       <c r="B3" s="38"/>
     </row>
-    <row r="4" spans="1:13" ht="228" customHeight="1">
+    <row r="4" spans="1:13" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="83" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C4" s="84"/>
       <c r="D4" s="84"/>
@@ -3474,16 +3639,16 @@
       <c r="G4" s="84"/>
       <c r="H4" s="40"/>
     </row>
-    <row r="5" spans="1:13" ht="24" customHeight="1"/>
-    <row r="6" spans="1:13" ht="12.75" customHeight="1">
+    <row r="5" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="42"/>
     </row>
-    <row r="7" spans="1:13" ht="42.75" customHeight="1">
+    <row r="7" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="43" t="s">
         <v>229</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
@@ -3491,12 +3656,12 @@
       <c r="G7" s="45"/>
       <c r="H7" s="46"/>
     </row>
-    <row r="8" spans="1:13" ht="36" customHeight="1">
+    <row r="8" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="43" t="s">
         <v>230</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
@@ -3504,7 +3669,7 @@
       <c r="G8" s="45"/>
       <c r="H8" s="46"/>
     </row>
-    <row r="9" spans="1:13" ht="31.5" customHeight="1">
+    <row r="9" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="43"/>
       <c r="C9" s="45"/>
       <c r="D9" s="45"/>
@@ -3513,10 +3678,10 @@
       <c r="G9" s="45"/>
       <c r="H9" s="46"/>
     </row>
-    <row r="10" spans="1:13" ht="30" customHeight="1">
+    <row r="10" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="42"/>
     </row>
-    <row r="11" spans="1:13" ht="29.25" customHeight="1">
+    <row r="11" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="43"/>
       <c r="C11" s="45"/>
       <c r="D11" s="45"/>
@@ -3525,7 +3690,7 @@
       <c r="G11" s="45"/>
       <c r="H11" s="46"/>
     </row>
-    <row r="12" spans="1:13" ht="30" customHeight="1">
+    <row r="12" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="43"/>
       <c r="C12" s="45"/>
       <c r="D12" s="45"/>
@@ -3534,7 +3699,7 @@
       <c r="G12" s="45"/>
       <c r="H12" s="46"/>
     </row>
-    <row r="13" spans="1:13" ht="20.25" customHeight="1">
+    <row r="13" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="43"/>
       <c r="C13" s="45"/>
       <c r="D13" s="45"/>
@@ -3543,7 +3708,7 @@
       <c r="G13" s="45"/>
       <c r="H13" s="46"/>
     </row>
-    <row r="14" spans="1:13" ht="30.75" customHeight="1">
+    <row r="14" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="43"/>
       <c r="C14" s="45"/>
       <c r="D14" s="45"/>
@@ -3552,7 +3717,7 @@
       <c r="G14" s="45"/>
       <c r="H14" s="46"/>
     </row>
-    <row r="15" spans="1:13" ht="46.5" customHeight="1">
+    <row r="15" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="43"/>
       <c r="C15" s="45"/>
       <c r="D15" s="45"/>
@@ -3561,7 +3726,7 @@
       <c r="G15" s="45"/>
       <c r="H15" s="46"/>
     </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1">
+    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="43"/>
       <c r="C16" s="45"/>
       <c r="D16" s="45"/>
@@ -3570,7 +3735,7 @@
       <c r="G16" s="45"/>
       <c r="H16" s="46"/>
     </row>
-    <row r="17" spans="2:8" ht="122.25" customHeight="1">
+    <row r="17" spans="2:8" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="43"/>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
@@ -3579,7 +3744,7 @@
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
     </row>
-    <row r="18" spans="2:8" ht="47.25" customHeight="1">
+    <row r="18" spans="2:8" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="43"/>
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
@@ -3588,7 +3753,7 @@
       <c r="G18" s="45"/>
       <c r="H18" s="46"/>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B57" s="39"/>
     </row>
   </sheetData>
@@ -3621,7 +3786,778 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K19"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
+        <v>236</v>
+      </c>
+      <c r="B1" s="88"/>
+    </row>
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="16" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="19"/>
+      <c r="H5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="73"/>
+      <c r="J5" s="73"/>
+      <c r="K5" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="J6" s="3"/>
+      <c r="K6" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="16" customFormat="1" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="16" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="73"/>
+      <c r="J9" s="73"/>
+      <c r="K9" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="15" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J18" s="3"/>
+      <c r="K18" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C19" s="71" t="s">
+        <v>325</v>
+      </c>
+      <c r="D19" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E19" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="23"/>
+      <c r="I19" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="J19" s="3"/>
+      <c r="K19" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{4DD40FF5-73A8-4DBF-8AF1-D1356D50C05B}" scale="75" showPageBreaks="1" fitToPage="1" printArea="1">
+      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
+      <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+      <pageSetup paperSize="9" scale="65" fitToHeight="5" orientation="landscape" r:id="rId1"/>
+      <headerFooter alignWithMargins="0">
+        <oddHeader>&amp;REntität: &amp;A</oddHeader>
+        <oddFooter>&amp;LData Dictionary Spezifikation SIP&amp;R&amp;8Seite &amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="5" orientation="landscape" r:id="rId2"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;REntität: &amp;A</oddHeader>
+    <oddFooter>&amp;LData Dictionary Archivische Ablieferungsschnittstelle (SIP)&amp;R&amp;8Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K6"/>
+  <sheetViews>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="F34" sqref="F34"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="87" t="s">
+        <v>237</v>
+      </c>
+      <c r="B1" s="88"/>
+    </row>
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>222</v>
+      </c>
+      <c r="K3" s="35" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>228</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>327</v>
+      </c>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{4DD40FF5-73A8-4DBF-8AF1-D1356D50C05B}" scale="75" showPageBreaks="1" fitToPage="1">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+      <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
+      <headerFooter alignWithMargins="0">
+        <oddHeader>&amp;REntität: &amp;A</oddHeader>
+        <oddFooter>&amp;LData Dictionary Spezifikation SIP&amp;R&amp;8Seite &amp;P</oddFooter>
+      </headerFooter>
+    </customSheetView>
+  </customSheetViews>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId2"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;REntität: &amp;A</oddHeader>
+    <oddFooter>&amp;LData Dictionary Archivische Ablieferungsschnittstelle (SIP)&amp;R&amp;8Seite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3633,7 +4569,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -3649,13 +4585,13 @@
     <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1">
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
         <v>238</v>
       </c>
       <c r="B1" s="88"/>
     </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -3690,7 +4626,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="25.5">
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>81</v>
       </c>
@@ -3698,7 +4634,7 @@
         <v>167</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -3721,15 +4657,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="65.25" customHeight="1">
+    <row r="5" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -3752,7 +4688,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="51">
+    <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>259</v>
       </c>
@@ -3781,9 +4717,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="15" customFormat="1" ht="38.25">
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>189</v>
@@ -3801,7 +4737,7 @@
         <v>204</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>40</v>
@@ -3812,9 +4748,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="15" customFormat="1" ht="25.5">
+    <row r="8" spans="1:11" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>190</v>
@@ -3843,9 +4779,9 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="15" customFormat="1" ht="106.5" customHeight="1">
+    <row r="9" spans="1:11" s="15" customFormat="1" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -3902,8 +4838,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3913,7 +4849,7 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="33.140625" style="47" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="47" customWidth="1"/>
@@ -4557,11 +5493,11 @@
     <col min="16140" max="16384" width="11.42578125" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="20.25">
-      <c r="A1" s="90" t="s">
-        <v>311</v>
-      </c>
-      <c r="B1" s="91"/>
+    <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="91" t="s">
+        <v>310</v>
+      </c>
+      <c r="B1" s="92"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -4572,7 +5508,7 @@
       <c r="J1" s="48"/>
       <c r="K1" s="48"/>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="49"/>
       <c r="B2" s="48"/>
       <c r="C2" s="48"/>
@@ -4585,7 +5521,7 @@
       <c r="J2" s="48"/>
       <c r="K2" s="48"/>
     </row>
-    <row r="3" spans="1:11" ht="25.5">
+    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -4620,15 +5556,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="25.5">
+    <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
+        <v>311</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="C4" s="71" t="s">
         <v>313</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>314</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>205</v>
@@ -4643,7 +5579,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I4" s="72"/>
       <c r="J4" s="72"/>
@@ -4651,15 +5587,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="25.5">
+    <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
+        <v>315</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>316</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="71" t="s">
         <v>317</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>318</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>205</v>
@@ -4680,15 +5616,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="38.25">
+    <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
+        <v>318</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>319</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="71" t="s">
         <v>320</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>321</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>205</v>
@@ -4709,15 +5645,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="29.25" customHeight="1">
+    <row r="7" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>323</v>
-      </c>
       <c r="C7" s="69" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>205</v>
@@ -4758,15 +5694,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
@@ -4774,199 +5710,199 @@
     <col min="4" max="4" width="11.42578125" style="76"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="54" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A1" s="97" t="s">
-        <v>376</v>
-      </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
+    <row r="1" spans="1:4" s="54" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="93" t="s">
+        <v>375</v>
+      </c>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
       <c r="D1" s="75"/>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1"/>
-    <row r="3" spans="1:4" ht="15">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="94" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" customHeight="1">
-      <c r="A4" s="98" t="s">
+      <c r="B4" s="94"/>
+      <c r="C4" s="94"/>
+    </row>
+    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="94" t="s">
         <v>373</v>
       </c>
-      <c r="B4" s="98"/>
-      <c r="C4" s="98"/>
-    </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1">
-      <c r="A5" s="98" t="s">
-        <v>374</v>
-      </c>
-      <c r="B5" s="98"/>
-      <c r="C5" s="98"/>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1"/>
-    <row r="7" spans="1:4" s="58" customFormat="1" ht="45" customHeight="1" thickBot="1">
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" s="58" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
-        <v>340</v>
-      </c>
-      <c r="B7" s="100" t="s">
-        <v>316</v>
-      </c>
-      <c r="C7" s="101"/>
+        <v>339</v>
+      </c>
+      <c r="B7" s="98" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="99"/>
       <c r="D7" s="77"/>
     </row>
-    <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1">
+    <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="95" t="s">
-        <v>341</v>
-      </c>
-      <c r="C8" s="96"/>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1">
+      <c r="B8" s="100" t="s">
+        <v>340</v>
+      </c>
+      <c r="C8" s="101"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="95" t="s">
-        <v>342</v>
-      </c>
-      <c r="C9" s="96"/>
-    </row>
-    <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1">
+      <c r="B9" s="100" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9" s="101"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="95" t="s">
-        <v>343</v>
-      </c>
-      <c r="C10" s="96"/>
-    </row>
-    <row r="11" spans="1:4" ht="45" customHeight="1">
+      <c r="B10" s="100" t="s">
+        <v>342</v>
+      </c>
+      <c r="C10" s="101"/>
+    </row>
+    <row r="11" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>217</v>
       </c>
       <c r="B11" s="102" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C11" s="103"/>
     </row>
-    <row r="12" spans="1:4" ht="30" customHeight="1">
+    <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
         <v>218</v>
       </c>
       <c r="B12" s="79" t="s">
+        <v>344</v>
+      </c>
+      <c r="C12" s="55" t="s">
         <v>345</v>
       </c>
-      <c r="C12" s="55" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1">
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="79" t="s">
+        <v>346</v>
+      </c>
+      <c r="C13" s="55" t="s">
         <v>347</v>
       </c>
-      <c r="C13" s="55" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30" customHeight="1" thickBot="1">
+    </row>
+    <row r="14" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="53"/>
       <c r="B14" s="80" t="s">
         <v>205</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="95" t="s">
-        <v>350</v>
-      </c>
-      <c r="C15" s="96"/>
-    </row>
-    <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1">
+      <c r="B15" s="100" t="s">
+        <v>349</v>
+      </c>
+      <c r="C15" s="101"/>
+    </row>
+    <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="95" t="s">
-        <v>351</v>
-      </c>
-      <c r="C16" s="96"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" thickBot="1">
+      <c r="B16" s="100" t="s">
+        <v>350</v>
+      </c>
+      <c r="C16" s="101"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="100" t="s">
+        <v>351</v>
+      </c>
+      <c r="C17" s="101"/>
+    </row>
+    <row r="18" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="57" t="s">
         <v>352</v>
       </c>
-      <c r="C17" s="96"/>
-    </row>
-    <row r="18" spans="1:4" ht="30" customHeight="1" thickBot="1">
-      <c r="A18" s="57" t="s">
+      <c r="B18" s="100" t="s">
         <v>353</v>
       </c>
-      <c r="B18" s="95" t="s">
-        <v>354</v>
-      </c>
-      <c r="C18" s="96"/>
-    </row>
-    <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1">
+      <c r="C18" s="101"/>
+    </row>
+    <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="100" t="s">
+        <v>354</v>
+      </c>
+      <c r="C19" s="101"/>
+    </row>
+    <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="s">
+        <v>376</v>
+      </c>
+      <c r="B20" s="100" t="s">
         <v>355</v>
       </c>
-      <c r="C19" s="96"/>
-    </row>
-    <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A20" s="50" t="s">
+      <c r="C20" s="101"/>
+    </row>
+    <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:4" s="58" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="61" t="s">
+        <v>374</v>
+      </c>
+      <c r="D22" s="77"/>
+    </row>
+    <row r="23" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="94" t="s">
         <v>377</v>
       </c>
-      <c r="B20" s="95" t="s">
-        <v>356</v>
-      </c>
-      <c r="C20" s="96"/>
-    </row>
-    <row r="21" spans="1:4" ht="30" customHeight="1"/>
-    <row r="22" spans="1:4" s="58" customFormat="1" ht="15">
-      <c r="A22" s="61" t="s">
-        <v>375</v>
-      </c>
-      <c r="D22" s="77"/>
-    </row>
-    <row r="23" spans="1:4" ht="60" customHeight="1">
-      <c r="A23" s="98" t="s">
+      <c r="B23" s="95"/>
+      <c r="C23" s="95"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="65" t="s">
         <v>378</v>
-      </c>
-      <c r="B23" s="99"/>
-      <c r="C23" s="99"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1"/>
-    <row r="25" spans="1:4" ht="15" thickBot="1">
-      <c r="A25" s="65" t="s">
-        <v>379</v>
       </c>
       <c r="B25" s="64"/>
       <c r="C25" s="64"/>
     </row>
-    <row r="26" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1">
+    <row r="26" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
+        <v>356</v>
+      </c>
+      <c r="B26" s="63" t="s">
         <v>357</v>
       </c>
-      <c r="B26" s="63" t="s">
+      <c r="C26" s="70" t="s">
         <v>358</v>
       </c>
-      <c r="C26" s="70" t="s">
-        <v>359</v>
-      </c>
       <c r="D26" s="77"/>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" thickBot="1">
+    <row r="27" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="57" t="s">
         <v>173</v>
       </c>
@@ -4974,10 +5910,10 @@
         <v>15</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" thickBot="1">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="57" t="s">
         <v>173</v>
       </c>
@@ -4985,10 +5921,10 @@
         <v>16</v>
       </c>
       <c r="C28" s="59" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" thickBot="1">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="57" t="s">
         <v>173</v>
       </c>
@@ -4996,10 +5932,10 @@
         <v>17</v>
       </c>
       <c r="C29" s="59" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" thickBot="1">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="57" t="s">
         <v>173</v>
       </c>
@@ -5007,148 +5943,159 @@
         <v>18</v>
       </c>
       <c r="C30" s="59" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C31" s="81"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="65" t="s">
+        <v>379</v>
+      </c>
+      <c r="C32" s="82"/>
+    </row>
+    <row r="33" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="62" t="s">
+        <v>356</v>
+      </c>
+      <c r="B33" s="63" t="s">
+        <v>357</v>
+      </c>
+      <c r="C33" s="70" t="s">
+        <v>358</v>
+      </c>
+      <c r="D33" s="77"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="96" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="96" t="s">
+        <v>205</v>
+      </c>
+      <c r="C34" s="55" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1">
-      <c r="C31" s="81"/>
-    </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1">
-      <c r="A32" s="65" t="s">
+      <c r="D34" s="78"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="97"/>
+      <c r="B35" s="97"/>
+      <c r="C35" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="D35" s="78"/>
+    </row>
+    <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="97"/>
+      <c r="B36" s="97"/>
+      <c r="C36" s="60" t="s">
         <v>380</v>
       </c>
-      <c r="C32" s="82"/>
-    </row>
-    <row r="33" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1">
-      <c r="A33" s="62" t="s">
-        <v>357</v>
-      </c>
-      <c r="B33" s="63" t="s">
-        <v>358</v>
-      </c>
-      <c r="C33" s="70" t="s">
-        <v>359</v>
-      </c>
-      <c r="D33" s="77"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1">
-      <c r="A34" s="92" t="s">
-        <v>74</v>
-      </c>
-      <c r="B34" s="92" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>364</v>
-      </c>
-      <c r="D34" s="78"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1">
-      <c r="A35" s="93"/>
-      <c r="B35" s="93"/>
-      <c r="C35" s="60" t="s">
+      <c r="D36" s="78"/>
+    </row>
+    <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="97"/>
+      <c r="B37" s="97"/>
+      <c r="C37" s="66" t="s">
+        <v>381</v>
+      </c>
+      <c r="D37" s="78"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="96"/>
+      <c r="C38" s="55" t="s">
         <v>365</v>
       </c>
-      <c r="D35" s="78"/>
-    </row>
-    <row r="36" spans="1:4" ht="67.5" customHeight="1">
-      <c r="A36" s="93"/>
-      <c r="B36" s="93"/>
-      <c r="C36" s="60" t="s">
-        <v>381</v>
-      </c>
-      <c r="D36" s="78"/>
-    </row>
-    <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1">
-      <c r="A37" s="93"/>
-      <c r="B37" s="93"/>
-      <c r="C37" s="66" t="s">
+      <c r="D38" s="78"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="97"/>
+      <c r="B39" s="97"/>
+      <c r="C39" s="60" t="s">
+        <v>366</v>
+      </c>
+      <c r="D39" s="78"/>
+    </row>
+    <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="97"/>
+      <c r="B40" s="97"/>
+      <c r="C40" s="60" t="s">
         <v>382</v>
       </c>
-      <c r="D37" s="78"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="92" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="92"/>
-      <c r="C38" s="55" t="s">
-        <v>366</v>
-      </c>
-      <c r="D38" s="78"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1">
-      <c r="A39" s="93"/>
-      <c r="B39" s="93"/>
-      <c r="C39" s="60" t="s">
+      <c r="D40" s="78"/>
+    </row>
+    <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="97"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="66" t="s">
+        <v>392</v>
+      </c>
+      <c r="D41" s="78"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="96" t="s">
         <v>367</v>
       </c>
-      <c r="D39" s="78"/>
-    </row>
-    <row r="40" spans="1:4" ht="63.75">
-      <c r="A40" s="93"/>
-      <c r="B40" s="93"/>
-      <c r="C40" s="60" t="s">
+      <c r="B42" s="96"/>
+      <c r="C42" s="55" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="97"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="60" t="s">
         <v>383</v>
       </c>
-      <c r="D40" s="78"/>
-    </row>
-    <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1">
-      <c r="A41" s="93"/>
-      <c r="B41" s="93"/>
-      <c r="C41" s="66" t="s">
-        <v>393</v>
-      </c>
-      <c r="D41" s="78"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" s="92" t="s">
-        <v>368</v>
-      </c>
-      <c r="B42" s="92"/>
-      <c r="C42" s="55" t="s">
+    </row>
+    <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="97"/>
+      <c r="B44" s="97"/>
+      <c r="C44" s="66" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="96" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="51">
-      <c r="A43" s="93"/>
-      <c r="B43" s="93"/>
-      <c r="C43" s="60" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1">
-      <c r="A44" s="93"/>
-      <c r="B44" s="93"/>
-      <c r="C44" s="66" t="s">
+      <c r="B45" s="96"/>
+      <c r="C45" s="67" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="97"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="60" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
-      <c r="A45" s="92" t="s">
-        <v>370</v>
-      </c>
-      <c r="B45" s="92"/>
-      <c r="C45" s="67" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="66" customHeight="1">
-      <c r="A46" s="93"/>
-      <c r="B46" s="93"/>
-      <c r="C46" s="60" t="s">
+    <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="104"/>
+      <c r="B47" s="104"/>
+      <c r="C47" s="68" t="s">
         <v>386</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="39" thickBot="1">
-      <c r="A47" s="94"/>
-      <c r="B47" s="94"/>
-      <c r="C47" s="68" t="s">
-        <v>387</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
@@ -5161,17 +6108,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5183,19 +6119,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="33.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.7109375" style="1" customWidth="1"/>
@@ -5210,13 +6146,13 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
         <v>231</v>
       </c>
       <c r="B1" s="86"/>
     </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -5251,7 +6187,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="38.25">
+    <row r="4" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>241</v>
       </c>
@@ -5282,7 +6218,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="63.75">
+    <row r="5" spans="1:11" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>242</v>
       </c>
@@ -5290,7 +6226,7 @@
         <v>132</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>205</v>
@@ -5313,7 +6249,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="51">
+    <row r="6" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>243</v>
       </c>
@@ -5344,7 +6280,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>244</v>
       </c>
@@ -5375,7 +6311,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="51">
+    <row r="8" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>245</v>
       </c>
@@ -5406,15 +6342,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="25.5">
+    <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>328</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="69" t="s">
         <v>330</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>331</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>205</v>
@@ -5426,10 +6362,10 @@
         <v>173</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H9" s="69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -5437,15 +6373,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="31.5" customHeight="1">
+    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="23" t="s">
         <v>334</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>335</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>20</v>
@@ -5454,7 +6390,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G10" s="69">
         <v>4</v>
@@ -5468,15 +6404,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="38.25">
+    <row r="11" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="71" t="s">
         <v>325</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>326</v>
       </c>
       <c r="D11" s="72" t="s">
         <v>223</v>
@@ -5526,7 +6462,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5535,10 +6471,10 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -5555,13 +6491,13 @@
     <col min="17" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="27" customHeight="1">
+    <row r="1" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="85" t="s">
         <v>232</v>
       </c>
       <c r="B1" s="86"/>
     </row>
-    <row r="3" spans="1:16" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:16" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -5596,7 +6532,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="82.5" customHeight="1">
+    <row r="4" spans="1:16" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>58</v>
       </c>
@@ -5604,7 +6540,7 @@
         <v>125</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>223</v>
@@ -5632,7 +6568,7 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="30.75" customHeight="1">
+    <row r="5" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>76</v>
       </c>
@@ -5668,7 +6604,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="53.25" customHeight="1">
+    <row r="6" spans="1:16" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>77</v>
       </c>
@@ -5676,7 +6612,7 @@
         <v>177</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -5704,7 +6640,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="89.25">
+    <row r="7" spans="1:16" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>78</v>
       </c>
@@ -5727,7 +6663,7 @@
         <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -5740,7 +6676,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:16" ht="107.25" customHeight="1">
+    <row r="8" spans="1:16" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>79</v>
       </c>
@@ -5756,7 +6692,7 @@
       <c r="E8" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="19" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="6"/>
@@ -5772,7 +6708,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="52.5" customHeight="1">
+    <row r="9" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>59</v>
       </c>
@@ -5780,7 +6716,7 @@
         <v>93</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>223</v>
@@ -5808,7 +6744,7 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:16" ht="94.5" customHeight="1">
+    <row r="10" spans="1:16" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>226</v>
       </c>
@@ -5844,7 +6780,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" ht="42" customHeight="1">
+    <row r="11" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>197</v>
       </c>
@@ -5852,7 +6788,7 @@
         <v>196</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>223</v>
@@ -5880,7 +6816,7 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
     </row>
-    <row r="12" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1">
+    <row r="12" spans="1:16" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>194</v>
       </c>
@@ -5888,7 +6824,7 @@
         <v>193</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>223</v>
@@ -5912,7 +6848,7 @@
       </c>
       <c r="L12" s="15"/>
     </row>
-    <row r="13" spans="1:16" ht="51">
+    <row r="13" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>60</v>
       </c>
@@ -5948,7 +6884,7 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
     </row>
-    <row r="14" spans="1:16" ht="102">
+    <row r="14" spans="1:16" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>80</v>
       </c>
@@ -5984,15 +6920,15 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
     </row>
-    <row r="15" spans="1:16" ht="38.25">
+    <row r="15" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="71" t="s">
         <v>325</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>326</v>
       </c>
       <c r="D15" s="72" t="s">
         <v>223</v>
@@ -6020,7 +6956,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -6054,19 +6990,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -6082,13 +7018,13 @@
     <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="20.25">
+    <row r="1" spans="1:15" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
         <v>239</v>
       </c>
       <c r="B1" s="88"/>
     </row>
-    <row r="3" spans="1:15" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:15" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -6123,7 +7059,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="120.75" customHeight="1">
+    <row r="4" spans="1:15" ht="120.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>246</v>
       </c>
@@ -6158,7 +7094,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="68.25" customHeight="1">
+    <row r="5" spans="1:15" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>248</v>
       </c>
@@ -6193,7 +7129,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="211.5" customHeight="1">
+    <row r="6" spans="1:15" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>247</v>
       </c>
@@ -6228,7 +7164,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="118.5" customHeight="1">
+    <row r="7" spans="1:15" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>249</v>
       </c>
@@ -6263,7 +7199,7 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="144" customHeight="1">
+    <row r="8" spans="1:15" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>250</v>
       </c>
@@ -6298,7 +7234,7 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="131.25" customHeight="1">
+    <row r="9" spans="1:15" ht="131.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>251</v>
       </c>
@@ -6333,7 +7269,7 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="25.5">
+    <row r="10" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>252</v>
       </c>
@@ -6364,7 +7300,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="60" customHeight="1">
+    <row r="11" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
         <v>253</v>
       </c>
@@ -6399,7 +7335,7 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" s="15" customFormat="1" ht="51">
+    <row r="12" spans="1:15" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>80</v>
       </c>
@@ -6430,13 +7366,13 @@
         <v>163</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -6469,7 +7405,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6478,10 +7414,10 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -6497,13 +7433,13 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1">
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
         <v>233</v>
       </c>
       <c r="B1" s="88"/>
     </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -6538,7 +7474,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="127.5">
+    <row r="4" spans="1:11" ht="127.5" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>81</v>
       </c>
@@ -6561,7 +7497,7 @@
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -6569,7 +7505,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="92.25" customHeight="1">
+    <row r="5" spans="1:11" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>254</v>
       </c>
@@ -6600,7 +7536,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="15" customFormat="1" ht="52.5" customHeight="1">
+    <row r="6" spans="1:11" s="15" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>255</v>
       </c>
@@ -6627,7 +7563,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="63" customHeight="1">
+    <row r="7" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>256</v>
       </c>
@@ -6650,7 +7586,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
@@ -6658,7 +7594,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="54.75" customHeight="1">
+    <row r="8" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>80</v>
       </c>
@@ -6689,15 +7625,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="54" customHeight="1">
+    <row r="9" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="71" t="s">
         <v>325</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>326</v>
       </c>
       <c r="D9" s="72" t="s">
         <v>223</v>
@@ -6747,7 +7683,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6759,7 +7695,7 @@
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -6776,13 +7712,13 @@
     <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="24.75" customHeight="1">
+    <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
         <v>234</v>
       </c>
       <c r="B1" s="89"/>
     </row>
-    <row r="3" spans="1:12" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:12" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -6817,7 +7753,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="106.5" customHeight="1">
+    <row r="4" spans="1:12" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>257</v>
       </c>
@@ -6848,7 +7784,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="68.25" customHeight="1">
+    <row r="5" spans="1:12" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>258</v>
       </c>
@@ -6879,7 +7815,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="27.75" customHeight="1">
+    <row r="6" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>259</v>
       </c>
@@ -6908,7 +7844,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="53.25" customHeight="1">
+    <row r="7" spans="1:12" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>260</v>
       </c>
@@ -6939,7 +7875,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="38.25">
+    <row r="8" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>197</v>
       </c>
@@ -6947,7 +7883,7 @@
         <v>196</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>223</v>
@@ -6971,7 +7907,7 @@
       </c>
       <c r="L8" s="15"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>194</v>
       </c>
@@ -6979,7 +7915,7 @@
         <v>193</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>223</v>
@@ -7003,7 +7939,7 @@
       </c>
       <c r="L9" s="15"/>
     </row>
-    <row r="10" spans="1:12" ht="144" customHeight="1">
+    <row r="10" spans="1:12" ht="144" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>261</v>
       </c>
@@ -7011,7 +7947,7 @@
         <v>175</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>223</v>
@@ -7034,7 +7970,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="76.5">
+    <row r="11" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>262</v>
       </c>
@@ -7042,7 +7978,7 @@
         <v>158</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>223</v>
@@ -7065,7 +8001,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="76.5">
+    <row r="12" spans="1:12" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>263</v>
       </c>
@@ -7073,7 +8009,7 @@
         <v>104</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>223</v>
@@ -7096,7 +8032,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="75.75" customHeight="1">
+    <row r="13" spans="1:12" ht="75.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>264</v>
       </c>
@@ -7104,7 +8040,7 @@
         <v>128</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>223</v>
@@ -7127,7 +8063,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="78" customHeight="1">
+    <row r="14" spans="1:12" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>265</v>
       </c>
@@ -7135,7 +8071,7 @@
         <v>191</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>223</v>
@@ -7158,7 +8094,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="54" customHeight="1">
+    <row r="15" spans="1:12" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>266</v>
       </c>
@@ -7189,15 +8125,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="55.5" customHeight="1">
+    <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="71" t="s">
         <v>325</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>326</v>
       </c>
       <c r="D16" s="72" t="s">
         <v>223</v>
@@ -7247,19 +8183,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L28"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="10" customWidth="1"/>
@@ -7276,13 +8212,13 @@
     <col min="13" max="16384" width="11.42578125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="23.25" customHeight="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
         <v>235</v>
       </c>
       <c r="B1" s="88"/>
     </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -7317,7 +8253,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="115.5" customHeight="1">
+    <row r="4" spans="1:11" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>267</v>
       </c>
@@ -7325,7 +8261,7 @@
         <v>156</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>20</v>
@@ -7348,7 +8284,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="140.1" customHeight="1">
+    <row r="5" spans="1:11" ht="140.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>268</v>
       </c>
@@ -7379,7 +8315,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="12" customFormat="1" ht="174" customHeight="1">
+    <row r="6" spans="1:11" s="12" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>258</v>
       </c>
@@ -7410,7 +8346,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="12" customFormat="1" ht="143.25" customHeight="1">
+    <row r="7" spans="1:11" s="12" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>269</v>
       </c>
@@ -7441,7 +8377,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="57" customHeight="1">
+    <row r="8" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>259</v>
       </c>
@@ -7470,7 +8406,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="74.25" customHeight="1">
+    <row r="9" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>270</v>
       </c>
@@ -7501,7 +8437,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="74.25" customHeight="1">
+    <row r="10" spans="1:11" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>271</v>
       </c>
@@ -7532,7 +8468,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="251.25" customHeight="1">
+    <row r="11" spans="1:11" ht="251.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>272</v>
       </c>
@@ -7563,7 +8499,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="51">
+    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>273</v>
       </c>
@@ -7594,7 +8530,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="52.5" customHeight="1">
+    <row r="13" spans="1:11" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>274</v>
       </c>
@@ -7621,7 +8557,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="31.5" customHeight="1">
+    <row r="14" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>275</v>
       </c>
@@ -7648,7 +8584,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="12" customFormat="1" ht="139.5" customHeight="1">
+    <row r="15" spans="1:11" s="12" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>79</v>
       </c>
@@ -7677,7 +8613,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="12" customFormat="1" ht="141.75" customHeight="1">
+    <row r="16" spans="1:11" s="12" customFormat="1" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>276</v>
       </c>
@@ -7708,7 +8644,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="38.25">
+    <row r="17" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>197</v>
       </c>
@@ -7716,7 +8652,7 @@
         <v>196</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D17" s="14" t="s">
         <v>223</v>
@@ -7740,7 +8676,7 @@
       </c>
       <c r="L17" s="15"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>194</v>
       </c>
@@ -7748,7 +8684,7 @@
         <v>193</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D18" s="14" t="s">
         <v>223</v>
@@ -7772,7 +8708,7 @@
       </c>
       <c r="L18" s="15"/>
     </row>
-    <row r="19" spans="1:12" ht="146.25" customHeight="1">
+    <row r="19" spans="1:12" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>261</v>
       </c>
@@ -7780,7 +8716,7 @@
         <v>175</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>223</v>
@@ -7803,7 +8739,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="63.75">
+    <row r="20" spans="1:12" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>262</v>
       </c>
@@ -7811,7 +8747,7 @@
         <v>158</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>223</v>
@@ -7834,7 +8770,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="90" customHeight="1">
+    <row r="21" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>263</v>
       </c>
@@ -7842,7 +8778,7 @@
         <v>104</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>223</v>
@@ -7865,7 +8801,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="75" customHeight="1">
+    <row r="22" spans="1:12" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>264</v>
       </c>
@@ -7873,7 +8809,7 @@
         <v>128</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>223</v>
@@ -7896,7 +8832,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:12" s="12" customFormat="1" ht="87" customHeight="1">
+    <row r="23" spans="1:12" s="12" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>265</v>
       </c>
@@ -7904,7 +8840,7 @@
         <v>191</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>223</v>
@@ -7927,7 +8863,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="12" customFormat="1" ht="87" customHeight="1">
+    <row r="24" spans="1:12" s="12" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>266</v>
       </c>
@@ -7958,11 +8894,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="88.5" customHeight="1">
+    <row r="25" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="B25" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="B25" s="19" t="s">
         <v>186</v>
       </c>
       <c r="C25" s="22" t="s">
@@ -7991,7 +8927,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="12" customFormat="1" ht="146.25" customHeight="1">
+    <row r="26" spans="1:12" s="12" customFormat="1" ht="146.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>80</v>
       </c>
@@ -8022,9 +8958,9 @@
         <v>163</v>
       </c>
     </row>
-    <row r="27" spans="1:12" s="1" customFormat="1" ht="25.5">
+    <row r="27" spans="1:12" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>183</v>
@@ -8053,15 +8989,15 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:12" s="1" customFormat="1" ht="53.25" customHeight="1">
+    <row r="28" spans="1:12" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="71" t="s">
         <v>325</v>
-      </c>
-      <c r="C28" s="71" t="s">
-        <v>326</v>
       </c>
       <c r="D28" s="72" t="s">
         <v>223</v>
@@ -8083,6 +9019,18 @@
       <c r="K28" s="25" t="s">
         <v>163</v>
       </c>
+    </row>
+    <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="90" t="s">
+        <v>420</v>
+      </c>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -8100,8 +9048,9 @@
       </headerFooter>
     </customSheetView>
   </customSheetViews>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A30:H30"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -8117,19 +9066,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -8145,13 +9094,13 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1">
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
-        <v>236</v>
+        <v>393</v>
       </c>
       <c r="B1" s="88"/>
     </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -8186,7 +9135,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="40.5" customHeight="1">
+    <row r="4" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>258</v>
       </c>
@@ -8194,22 +9143,22 @@
         <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>120</v>
+        <v>398</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
+      <c r="E4" s="27" t="s">
+        <v>205</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>173</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>302</v>
+        <v>401</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -8217,482 +9166,105 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="16" customFormat="1" ht="25.5">
+    <row r="5" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="19" t="s">
+        <v>394</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
       <c r="K5" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>279</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>121</v>
+        <v>396</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>400</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>223</v>
+      <c r="E6" s="27" t="s">
+        <v>205</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G6" s="23" t="s">
-        <v>18</v>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>105</v>
+        <v>403</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>166</v>
+        <v>203</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="16" customFormat="1" ht="210" customHeight="1">
+      <c r="K6" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>270</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>118</v>
+        <v>422</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>423</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
+        <v>424</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="25.5">
-      <c r="A8" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="16" customFormat="1" ht="58.5" customHeight="1">
-      <c r="A9" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="73"/>
-      <c r="J9" s="73"/>
-      <c r="K9" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="44.25" customHeight="1">
-      <c r="A10" s="32" t="s">
-        <v>282</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="145.5" customHeight="1">
-      <c r="A11" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>223</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="51">
-      <c r="A12" s="32" t="s">
-        <v>262</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="72.75" customHeight="1">
-      <c r="A13" s="32" t="s">
-        <v>263</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="63" customHeight="1">
-      <c r="A14" s="32" t="s">
-        <v>264</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="15" customFormat="1" ht="63.75">
-      <c r="A15" s="32" t="s">
-        <v>265</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="42" customHeight="1">
-      <c r="A16" s="32" t="s">
-        <v>266</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="67.5" customHeight="1">
-      <c r="A17" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="25.5">
-      <c r="A18" s="32" t="s">
-        <v>278</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="54.75" customHeight="1">
-      <c r="A19" s="32" t="s">
-        <v>324</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>326</v>
-      </c>
-      <c r="D19" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="E19" s="72" t="s">
-        <v>223</v>
-      </c>
-      <c r="F19" s="25" t="s">
-        <v>173</v>
-      </c>
-      <c r="G19" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="23"/>
-      <c r="I19" s="72" t="s">
-        <v>166</v>
-      </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="25" t="s">
-        <v>163</v>
-      </c>
-    </row>
   </sheetData>
-  <customSheetViews>
-    <customSheetView guid="{4DD40FF5-73A8-4DBF-8AF1-D1356D50C05B}" scale="75" showPageBreaks="1" fitToPage="1" printArea="1">
-      <pane ySplit="3" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD19"/>
-      <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
-      <pageSetup paperSize="9" scale="65" fitToHeight="5" orientation="landscape" r:id="rId1"/>
-      <headerFooter alignWithMargins="0">
-        <oddHeader>&amp;REntität: &amp;A</oddHeader>
-        <oddFooter>&amp;LData Dictionary Spezifikation SIP&amp;R&amp;8Seite &amp;P</oddFooter>
-      </headerFooter>
-    </customSheetView>
-  </customSheetViews>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="65" fitToHeight="5" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="5" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;REntität: &amp;A</oddHeader>
     <oddFooter>&amp;LData Dictionary Archivische Ablieferungsschnittstelle (SIP)&amp;R&amp;8Seite &amp;P</oddFooter>
@@ -8701,19 +9273,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.140625" style="13" customWidth="1"/>
     <col min="2" max="2" width="33.140625" style="1" customWidth="1"/>
@@ -8729,13 +9301,13 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" customHeight="1">
+    <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
-        <v>237</v>
+        <v>404</v>
       </c>
       <c r="B1" s="88"/>
     </row>
-    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5">
+    <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
         <v>81</v>
       </c>
@@ -8770,116 +9342,225 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="63.75">
+    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>228</v>
+        <v>405</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>411</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="E4" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
+        <v>418</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
       <c r="K4" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="95.25" customHeight="1">
+    <row r="5" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>327</v>
+        <v>408</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>412</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="E5" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J5" s="3"/>
+      <c r="K5" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19" t="s">
+      <c r="H6" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>396</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>422</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="6" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="64.5" customHeight="1">
-      <c r="A6" s="32" t="s">
-        <v>259</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
   </sheetData>
-  <customSheetViews>
-    <customSheetView guid="{4DD40FF5-73A8-4DBF-8AF1-D1356D50C05B}" scale="75" showPageBreaks="1" fitToPage="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
-      <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
-      <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId1"/>
-      <headerFooter alignWithMargins="0">
-        <oddHeader>&amp;REntität: &amp;A</oddHeader>
-        <oddFooter>&amp;LData Dictionary Spezifikation SIP&amp;R&amp;8Seite &amp;P</oddFooter>
-      </headerFooter>
-    </customSheetView>
-  </customSheetViews>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="65" orientation="landscape" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="5" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;REntität: &amp;A</oddHeader>
     <oddFooter>&amp;LData Dictionary Archivische Ablieferungsschnittstelle (SIP)&amp;R&amp;8Seite &amp;P</oddFooter>

</xml_diff>

<commit_message>
Synchronisation von XSD Schema und Data Dictionary
</commit_message>
<xml_diff>
--- a/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
+++ b/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\eCH\Fachgruppe_Digitale_Archivierung\eCH-0160 Archivische Ablieferungsschnittstelle (SIP)\v1.1\03_Dokumentation\2_Entwurf_v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\eCH\Fachgruppe_Digitale_Archivierung\eCH-0160\v1.1\05_Entwurf_v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Titelblatt" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="426">
   <si>
     <t xml:space="preserve">Systeme, die mit dem beschriebenen System Daten ausgetauscht haben und damit Subsysteme, Parallelsysteme oder übergeordnete Systeme sind. Hier werden die Bezeichnungen der Systeme und die Art der Verwandtschaft eingetragen. </t>
   </si>
@@ -1063,9 +1063,6 @@
     <t xml:space="preserve">Angabe, ob es sich beim Dokument zum Zeitpunkt der Ablieferung um ein digitales Dokument, oder um ein nicht-digitales Dokument handelt (Papier, audiovisuell). Ein Dokument kann nur einer der beiden Erscheinungsformen (entweder digital oder nicht-digital) zugewiesen werden. Dokumente, die vor der Ablieferung aus einem digitalen und einem nicht-digitalen Teil bestanden, müssen als zwei getrennte Dokumente abgeliefert werden. </t>
   </si>
   <si>
-    <t xml:space="preserve">Die Ablieferungsnummer dient zur Identifizierung der Ablieferung im Archiv Sie besteht aus dem Ablieferungsjahr und einer Laufnummer innerhalb dieses Jahres. </t>
-  </si>
-  <si>
     <t>Die vom Archiv vergebene Nummer des Angebots, auf welches sich die Ablieferung stützt.</t>
   </si>
   <si>
@@ -1161,10 +1158,6 @@
   </si>
   <si>
     <t>text (token)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aktenzeichen des Übernahmedossiers
-</t>
   </si>
   <si>
     <t>März 2012</t>
@@ -1613,6 +1606,13 @@
   </si>
   <si>
     <t>Ordnungszahl welche die Reihenfolge von Aktivitäten innerhalb eines Dossiers festlegt, muss innerhalb des selben Vorgangs eindeutig sein.</t>
+  </si>
+  <si>
+    <t>Die Ablieferungsnummer dient zur Identifizierung der Ablieferung im Archiv. Sie besteht in der Regel aus dem Ablieferungsjahr und einer Laufnummer innerhalb dieses Jahres. Die Ablieferungsnummer kann auch Buchstaben enthalten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aktenzeichen des Übernahmedossiers des Archivs
+</t>
   </si>
 </sst>
 </file>
@@ -2289,6 +2289,21 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2298,31 +2313,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3648,7 +3648,7 @@
         <v>229</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
@@ -3661,7 +3661,7 @@
         <v>230</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
@@ -3795,7 +3795,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4095,7 +4095,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>262</v>
       </c>
@@ -4126,7 +4126,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>263</v>
       </c>
@@ -4314,13 +4314,13 @@
     </row>
     <row r="19" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="71" t="s">
         <v>324</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>325</v>
       </c>
       <c r="D19" s="72" t="s">
         <v>223</v>
@@ -4478,7 +4478,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -4493,7 +4493,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -4566,7 +4566,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4634,7 +4634,7 @@
         <v>167</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -4665,7 +4665,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -4737,7 +4737,7 @@
         <v>204</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>40</v>
@@ -4846,7 +4846,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5495,7 +5495,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="91" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B1" s="92"/>
       <c r="C1" s="48"/>
@@ -5558,13 +5558,13 @@
     </row>
     <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="C4" s="71" t="s">
         <v>312</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>313</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>205</v>
@@ -5579,7 +5579,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I4" s="72"/>
       <c r="J4" s="72"/>
@@ -5589,13 +5589,13 @@
     </row>
     <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
+        <v>314</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>315</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="71" t="s">
         <v>316</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>317</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>205</v>
@@ -5618,13 +5618,13 @@
     </row>
     <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>318</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="71" t="s">
         <v>319</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>320</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>205</v>
@@ -5647,13 +5647,13 @@
     </row>
     <row r="7" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
+        <v>320</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>321</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>322</v>
-      </c>
       <c r="C7" s="69" t="s">
-        <v>336</v>
+        <v>425</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>205</v>
@@ -5711,98 +5711,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="54" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
-        <v>375</v>
-      </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="93"/>
+      <c r="A1" s="98" t="s">
+        <v>373</v>
+      </c>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
       <c r="D1" s="75"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="99" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+    </row>
+    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="99" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="94" t="s">
-        <v>372</v>
-      </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="94"/>
-    </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="94" t="s">
-        <v>373</v>
-      </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="99"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" s="58" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="B7" s="98" t="s">
-        <v>315</v>
-      </c>
-      <c r="C7" s="99"/>
+        <v>337</v>
+      </c>
+      <c r="B7" s="101" t="s">
+        <v>314</v>
+      </c>
+      <c r="C7" s="102"/>
       <c r="D7" s="77"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="100" t="s">
-        <v>340</v>
-      </c>
-      <c r="C8" s="101"/>
+      <c r="B8" s="96" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" s="97"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="100" t="s">
-        <v>341</v>
-      </c>
-      <c r="C9" s="101"/>
+      <c r="B9" s="96" t="s">
+        <v>339</v>
+      </c>
+      <c r="C9" s="97"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="100" t="s">
-        <v>342</v>
-      </c>
-      <c r="C10" s="101"/>
+      <c r="B10" s="96" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" s="97"/>
     </row>
     <row r="11" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="102" t="s">
-        <v>343</v>
-      </c>
-      <c r="C11" s="103"/>
+      <c r="B11" s="103" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" s="104"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
         <v>218</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="79" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5811,94 +5811,94 @@
         <v>205</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="100" t="s">
-        <v>349</v>
-      </c>
-      <c r="C15" s="101"/>
+      <c r="B15" s="96" t="s">
+        <v>347</v>
+      </c>
+      <c r="C15" s="97"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="100" t="s">
-        <v>350</v>
-      </c>
-      <c r="C16" s="101"/>
+      <c r="B16" s="96" t="s">
+        <v>348</v>
+      </c>
+      <c r="C16" s="97"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="100" t="s">
-        <v>351</v>
-      </c>
-      <c r="C17" s="101"/>
+      <c r="B17" s="96" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" s="97"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
-        <v>352</v>
-      </c>
-      <c r="B18" s="100" t="s">
-        <v>353</v>
-      </c>
-      <c r="C18" s="101"/>
+        <v>350</v>
+      </c>
+      <c r="B18" s="96" t="s">
+        <v>351</v>
+      </c>
+      <c r="C18" s="97"/>
     </row>
     <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="100" t="s">
-        <v>354</v>
-      </c>
-      <c r="C19" s="101"/>
+      <c r="B19" s="96" t="s">
+        <v>352</v>
+      </c>
+      <c r="C19" s="97"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>376</v>
-      </c>
-      <c r="B20" s="100" t="s">
-        <v>355</v>
-      </c>
-      <c r="C20" s="101"/>
+        <v>374</v>
+      </c>
+      <c r="B20" s="96" t="s">
+        <v>353</v>
+      </c>
+      <c r="C20" s="97"/>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:4" s="58" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="61" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D22" s="77"/>
     </row>
     <row r="23" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="94" t="s">
-        <v>377</v>
-      </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
+      <c r="A23" s="99" t="s">
+        <v>375</v>
+      </c>
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="65" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B25" s="64"/>
       <c r="C25" s="64"/>
     </row>
     <row r="26" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
+        <v>354</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>355</v>
+      </c>
+      <c r="C26" s="70" t="s">
         <v>356</v>
-      </c>
-      <c r="B26" s="63" t="s">
-        <v>357</v>
-      </c>
-      <c r="C26" s="70" t="s">
-        <v>358</v>
       </c>
       <c r="D26" s="77"/>
     </row>
@@ -5910,7 +5910,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5921,7 +5921,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="59" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5932,7 +5932,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="59" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5943,7 +5943,7 @@
         <v>18</v>
       </c>
       <c r="C30" s="59" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5951,151 +5951,140 @@
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="65" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="C32" s="82"/>
     </row>
     <row r="33" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
+        <v>354</v>
+      </c>
+      <c r="B33" s="63" t="s">
+        <v>355</v>
+      </c>
+      <c r="C33" s="70" t="s">
         <v>356</v>
       </c>
-      <c r="B33" s="63" t="s">
-        <v>357</v>
-      </c>
-      <c r="C33" s="70" t="s">
-        <v>358</v>
-      </c>
       <c r="D33" s="77"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="96" t="s">
+      <c r="A34" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="96" t="s">
+      <c r="B34" s="93" t="s">
         <v>205</v>
       </c>
       <c r="C34" s="55" t="s">
+        <v>361</v>
+      </c>
+      <c r="D34" s="78"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="94"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="60" t="s">
+        <v>362</v>
+      </c>
+      <c r="D35" s="78"/>
+    </row>
+    <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="94"/>
+      <c r="B36" s="94"/>
+      <c r="C36" s="60" t="s">
+        <v>378</v>
+      </c>
+      <c r="D36" s="78"/>
+    </row>
+    <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="66" t="s">
+        <v>379</v>
+      </c>
+      <c r="D37" s="78"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="93" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="93"/>
+      <c r="C38" s="55" t="s">
         <v>363</v>
       </c>
-      <c r="D34" s="78"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="97"/>
-      <c r="B35" s="97"/>
-      <c r="C35" s="60" t="s">
+      <c r="D38" s="78"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="94"/>
+      <c r="B39" s="94"/>
+      <c r="C39" s="60" t="s">
         <v>364</v>
       </c>
-      <c r="D35" s="78"/>
-    </row>
-    <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="97"/>
-      <c r="B36" s="97"/>
-      <c r="C36" s="60" t="s">
+      <c r="D39" s="78"/>
+    </row>
+    <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="94"/>
+      <c r="B40" s="94"/>
+      <c r="C40" s="60" t="s">
         <v>380</v>
       </c>
-      <c r="D36" s="78"/>
-    </row>
-    <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="97"/>
-      <c r="B37" s="97"/>
-      <c r="C37" s="66" t="s">
+      <c r="D40" s="78"/>
+    </row>
+    <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="94"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="66" t="s">
+        <v>390</v>
+      </c>
+      <c r="D41" s="78"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="93" t="s">
+        <v>365</v>
+      </c>
+      <c r="B42" s="93"/>
+      <c r="C42" s="55" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="94"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="D37" s="78"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="96" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="96"/>
-      <c r="C38" s="55" t="s">
-        <v>365</v>
-      </c>
-      <c r="D38" s="78"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="97"/>
-      <c r="B39" s="97"/>
-      <c r="C39" s="60" t="s">
-        <v>366</v>
-      </c>
-      <c r="D39" s="78"/>
-    </row>
-    <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="97"/>
-      <c r="B40" s="97"/>
-      <c r="C40" s="60" t="s">
+    </row>
+    <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="94"/>
+      <c r="B44" s="94"/>
+      <c r="C44" s="66" t="s">
         <v>382</v>
       </c>
-      <c r="D40" s="78"/>
-    </row>
-    <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="97"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="66" t="s">
-        <v>392</v>
-      </c>
-      <c r="D41" s="78"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="96" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="93" t="s">
         <v>367</v>
       </c>
-      <c r="B42" s="96"/>
-      <c r="C42" s="55" t="s">
+      <c r="B45" s="93"/>
+      <c r="C45" s="67" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="97"/>
-      <c r="B43" s="97"/>
-      <c r="C43" s="60" t="s">
+    <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="94"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="60" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="97"/>
-      <c r="B44" s="97"/>
-      <c r="C44" s="66" t="s">
+    <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="95"/>
+      <c r="B47" s="95"/>
+      <c r="C47" s="68" t="s">
         <v>384</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="96" t="s">
-        <v>369</v>
-      </c>
-      <c r="B45" s="96"/>
-      <c r="C45" s="67" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="97"/>
-      <c r="B46" s="97"/>
-      <c r="C46" s="60" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="104"/>
-      <c r="B47" s="104"/>
-      <c r="C47" s="68" t="s">
-        <v>386</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
@@ -6108,6 +6097,17 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6226,7 +6226,7 @@
         <v>132</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>205</v>
@@ -6344,13 +6344,13 @@
     </row>
     <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="69" t="s">
         <v>329</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>330</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>205</v>
@@ -6362,10 +6362,10 @@
         <v>173</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H9" s="69" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -6375,13 +6375,13 @@
     </row>
     <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="23" t="s">
         <v>333</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>334</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>20</v>
@@ -6390,7 +6390,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G10" s="69">
         <v>4</v>
@@ -6406,13 +6406,13 @@
     </row>
     <row r="11" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="71" t="s">
         <v>324</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>325</v>
       </c>
       <c r="D11" s="72" t="s">
         <v>223</v>
@@ -6468,10 +6468,10 @@
   </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6532,7 +6532,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>58</v>
       </c>
@@ -6540,7 +6540,7 @@
         <v>125</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>303</v>
+        <v>424</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>223</v>
@@ -6612,7 +6612,7 @@
         <v>177</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -6663,7 +6663,7 @@
         <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
@@ -6708,7 +6708,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>59</v>
       </c>
@@ -6716,7 +6716,7 @@
         <v>93</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>223</v>
@@ -6824,7 +6824,7 @@
         <v>193</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>223</v>
@@ -6922,13 +6922,13 @@
     </row>
     <row r="15" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="71" t="s">
         <v>324</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>325</v>
       </c>
       <c r="D15" s="72" t="s">
         <v>223</v>
@@ -6999,7 +6999,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7627,13 +7627,13 @@
     </row>
     <row r="9" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="71" t="s">
         <v>324</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>325</v>
       </c>
       <c r="D9" s="72" t="s">
         <v>223</v>
@@ -7690,9 +7690,9 @@
   <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8127,13 +8127,13 @@
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="71" t="s">
         <v>324</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>325</v>
       </c>
       <c r="D16" s="72" t="s">
         <v>223</v>
@@ -8190,9 +8190,9 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8261,7 +8261,7 @@
         <v>156</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>20</v>
@@ -8778,7 +8778,7 @@
         <v>104</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>223</v>
@@ -8896,7 +8896,7 @@
     </row>
     <row r="25" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>186</v>
@@ -8991,13 +8991,13 @@
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="71" t="s">
         <v>324</v>
-      </c>
-      <c r="C28" s="71" t="s">
-        <v>325</v>
       </c>
       <c r="D28" s="72" t="s">
         <v>223</v>
@@ -9022,7 +9022,7 @@
     </row>
     <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="90" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B30" s="90"/>
       <c r="C30" s="90"/>
@@ -9075,7 +9075,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7:XFD7"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9096,7 +9096,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B1" s="88"/>
     </row>
@@ -9143,7 +9143,7 @@
         <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -9155,10 +9155,10 @@
         <v>173</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -9168,13 +9168,13 @@
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -9189,7 +9189,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -9199,13 +9199,13 @@
     </row>
     <row r="6" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -9217,10 +9217,10 @@
         <v>173</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>203</v>
@@ -9232,13 +9232,13 @@
     </row>
     <row r="7" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
+        <v>420</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>422</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>424</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>223</v>
@@ -9279,10 +9279,10 @@
   </sheetPr>
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="I32"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9303,7 +9303,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="87" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B1" s="88"/>
     </row>
@@ -9344,13 +9344,13 @@
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -9362,10 +9362,10 @@
         <v>173</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -9375,13 +9375,13 @@
     </row>
     <row r="5" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -9393,10 +9393,10 @@
         <v>173</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>203</v>
@@ -9408,13 +9408,13 @@
     </row>
     <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -9429,7 +9429,7 @@
         <v>18</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -9445,7 +9445,7 @@
         <v>160</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>223</v>
@@ -9456,9 +9456,7 @@
       <c r="F7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="3" t="s">
         <v>203</v>
@@ -9470,13 +9468,13 @@
     </row>
     <row r="8" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>223</v>
@@ -9488,7 +9486,7 @@
         <v>173</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
@@ -9505,7 +9503,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>223</v>
@@ -9528,13 +9526,13 @@
     </row>
     <row r="10" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>423</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>425</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
Metadaten in Vorgang und Aktivität in Schema eingefügt
</commit_message>
<xml_diff>
--- a/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
+++ b/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Titelblatt" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="0" hidden="1">Titelblatt!$A:$A,Titelblatt!$4:$5</definedName>
     <definedName name="Z_4DD40FF5_73A8_4DBF_8AF1_D1356D50C05B_.wvu.PrintTitles" localSheetId="7" hidden="1">Vorgang!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
   <customWorkbookViews>
     <customWorkbookView name="Georg Büchler - Persönliche Ansicht" guid="{4DD40FF5-73A8-4DBF-8AF1-D1356D50C05B}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1676" windowHeight="821" tabRatio="573" activeSheetId="9"/>
   </customWorkbookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="429">
   <si>
     <t xml:space="preserve">Systeme, die mit dem beschriebenen System Daten ausgetauscht haben und damit Subsysteme, Parallelsysteme oder übergeordnete Systeme sind. Hier werden die Bezeichnungen der Systeme und die Art der Verwandtschaft eingetragen. </t>
   </si>
@@ -1523,27 +1523,9 @@
     <t>vorschreibung</t>
   </si>
   <si>
-    <t>akteur</t>
-  </si>
-  <si>
-    <t>Akteur</t>
-  </si>
-  <si>
-    <t>abschlussvermerk</t>
-  </si>
-  <si>
-    <t>Abschlussvermerk</t>
-  </si>
-  <si>
-    <t>Beschreibung der Tätigkeit, die ausgeführt werden soll.</t>
-  </si>
-  <si>
     <t>Akteur, welcher die Aktivität durchführt. Im Organigramm bzw. den Organisationsvorschriften der Verwaltungseinheit aufgeführte Rollen bzw. Personen.</t>
   </si>
   <si>
-    <t>Kurze Beschreibung des Ergebnisses der Aktivität.</t>
-  </si>
-  <si>
     <t>Tag, an dem die Aktivität abgeschlossen worden ist.</t>
   </si>
   <si>
@@ -1557,9 +1539,6 @@
   </si>
   <si>
     <t>Dossier anlegen</t>
-  </si>
-  <si>
-    <t>Alle notwendigen Dokumente angelegt</t>
   </si>
   <si>
     <r>
@@ -1613,6 +1592,36 @@
   <si>
     <t xml:space="preserve">Aktenzeichen des Übernahmedossiers des Archivs
 </t>
+  </si>
+  <si>
+    <t>Federführung</t>
+  </si>
+  <si>
+    <t>federfuerung</t>
+  </si>
+  <si>
+    <t>Akteur, der für die korrekte Durchführung des Geschäftsvorfalls verantwortlich ist.</t>
+  </si>
+  <si>
+    <t>Ergänzende Information zum Vorgang.</t>
+  </si>
+  <si>
+    <t>Kantonale Impfkoordination</t>
+  </si>
+  <si>
+    <t>Anweisung</t>
+  </si>
+  <si>
+    <t>anweisung</t>
+  </si>
+  <si>
+    <t>Beschreibung der Tätigkeit, die ausgeführt werden soll. Für die Vorschreibungen sollen entsprechende Standardanweisungen hinterlegt werden</t>
+  </si>
+  <si>
+    <t>Freitext für die Eingabe der Anweisung zu einer Aktivität.</t>
+  </si>
+  <si>
+    <t>Geschäftsart - Differenzbereinigung</t>
   </si>
 </sst>
 </file>
@@ -2032,7 +2041,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2257,6 +2266,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -3629,14 +3641,14 @@
       <c r="B3" s="38"/>
     </row>
     <row r="4" spans="1:13" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="84" t="s">
         <v>286</v>
       </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
       <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:13" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3795,7 +3807,7 @@
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3815,10 +3827,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -4399,10 +4411,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>237</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -4586,10 +4598,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>238</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -5494,10 +5506,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="92" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="92"/>
+      <c r="B1" s="93"/>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
       <c r="E1" s="48"/>
@@ -5653,7 +5665,7 @@
         <v>321</v>
       </c>
       <c r="C7" s="69" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>205</v>
@@ -5699,7 +5711,7 @@
   <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5711,11 +5723,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="54" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="99" t="s">
         <v>373</v>
       </c>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="75"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5725,65 +5737,65 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="100" t="s">
         <v>370</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
     </row>
     <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="100" t="s">
         <v>371</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" s="58" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="102" t="s">
         <v>314</v>
       </c>
-      <c r="C7" s="102"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="77"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="97" t="s">
         <v>338</v>
       </c>
-      <c r="C8" s="97"/>
+      <c r="C8" s="98"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="97" t="s">
         <v>339</v>
       </c>
-      <c r="C9" s="97"/>
+      <c r="C9" s="98"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="97" t="s">
         <v>340</v>
       </c>
-      <c r="C10" s="97"/>
+      <c r="C10" s="98"/>
     </row>
     <row r="11" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="104" t="s">
         <v>341</v>
       </c>
-      <c r="C11" s="104"/>
+      <c r="C11" s="105"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
@@ -5818,55 +5830,55 @@
       <c r="A15" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="97" t="s">
         <v>347</v>
       </c>
-      <c r="C15" s="97"/>
+      <c r="C15" s="98"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="97" t="s">
         <v>348</v>
       </c>
-      <c r="C16" s="97"/>
+      <c r="C16" s="98"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="97" t="s">
         <v>349</v>
       </c>
-      <c r="C17" s="97"/>
+      <c r="C17" s="98"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
         <v>350</v>
       </c>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="97" t="s">
         <v>351</v>
       </c>
-      <c r="C18" s="97"/>
+      <c r="C18" s="98"/>
     </row>
     <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="97" t="s">
         <v>352</v>
       </c>
-      <c r="C19" s="97"/>
+      <c r="C19" s="98"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>374</v>
       </c>
-      <c r="B20" s="96" t="s">
+      <c r="B20" s="97" t="s">
         <v>353</v>
       </c>
-      <c r="C20" s="97"/>
+      <c r="C20" s="98"/>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:4" s="58" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5876,11 +5888,11 @@
       <c r="D22" s="77"/>
     </row>
     <row r="23" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="99" t="s">
+      <c r="A23" s="100" t="s">
         <v>375</v>
       </c>
-      <c r="B23" s="100"/>
-      <c r="C23" s="100"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -5968,10 +5980,10 @@
       <c r="D33" s="77"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="93" t="s">
+      <c r="A34" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="93" t="s">
+      <c r="B34" s="94" t="s">
         <v>205</v>
       </c>
       <c r="C34" s="55" t="s">
@@ -5980,105 +5992,105 @@
       <c r="D34" s="78"/>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="94"/>
-      <c r="B35" s="94"/>
+      <c r="A35" s="95"/>
+      <c r="B35" s="95"/>
       <c r="C35" s="60" t="s">
         <v>362</v>
       </c>
       <c r="D35" s="78"/>
     </row>
     <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="94"/>
-      <c r="B36" s="94"/>
+      <c r="A36" s="95"/>
+      <c r="B36" s="95"/>
       <c r="C36" s="60" t="s">
         <v>378</v>
       </c>
       <c r="D36" s="78"/>
     </row>
     <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="94"/>
-      <c r="B37" s="94"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="66" t="s">
         <v>379</v>
       </c>
       <c r="D37" s="78"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="93" t="s">
+      <c r="A38" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="93"/>
+      <c r="B38" s="94"/>
       <c r="C38" s="55" t="s">
         <v>363</v>
       </c>
       <c r="D38" s="78"/>
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="94"/>
-      <c r="B39" s="94"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="95"/>
       <c r="C39" s="60" t="s">
         <v>364</v>
       </c>
       <c r="D39" s="78"/>
     </row>
     <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="94"/>
-      <c r="B40" s="94"/>
+      <c r="A40" s="95"/>
+      <c r="B40" s="95"/>
       <c r="C40" s="60" t="s">
         <v>380</v>
       </c>
       <c r="D40" s="78"/>
     </row>
     <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="94"/>
-      <c r="B41" s="94"/>
+      <c r="A41" s="95"/>
+      <c r="B41" s="95"/>
       <c r="C41" s="66" t="s">
         <v>390</v>
       </c>
       <c r="D41" s="78"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="94" t="s">
         <v>365</v>
       </c>
-      <c r="B42" s="93"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="55" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="94"/>
-      <c r="B43" s="94"/>
+      <c r="A43" s="95"/>
+      <c r="B43" s="95"/>
       <c r="C43" s="60" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="94"/>
-      <c r="B44" s="94"/>
+      <c r="A44" s="95"/>
+      <c r="B44" s="95"/>
       <c r="C44" s="66" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="93" t="s">
+      <c r="A45" s="94" t="s">
         <v>367</v>
       </c>
-      <c r="B45" s="93"/>
+      <c r="B45" s="94"/>
       <c r="C45" s="67" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="94"/>
-      <c r="B46" s="94"/>
+      <c r="A46" s="95"/>
+      <c r="B46" s="95"/>
       <c r="C46" s="60" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="95"/>
-      <c r="B47" s="95"/>
+      <c r="A47" s="96"/>
+      <c r="B47" s="96"/>
       <c r="C47" s="68" t="s">
         <v>384</v>
       </c>
@@ -6147,10 +6159,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>231</v>
       </c>
-      <c r="B1" s="86"/>
+      <c r="B1" s="87"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -6468,7 +6480,7 @@
   </sheetPr>
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
@@ -6492,10 +6504,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="86"/>
+      <c r="B1" s="87"/>
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -6540,7 +6552,7 @@
         <v>125</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>223</v>
@@ -7019,10 +7031,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>239</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:15" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -7434,10 +7446,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -7713,10 +7725,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>234</v>
       </c>
-      <c r="B1" s="89"/>
+      <c r="B1" s="90"/>
     </row>
     <row r="3" spans="1:12" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -8190,9 +8202,9 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="50" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8213,10 +8225,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -8896,7 +8908,7 @@
     </row>
     <row r="25" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>186</v>
@@ -9021,16 +9033,16 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="90" t="s">
-        <v>418</v>
-      </c>
-      <c r="B30" s="90"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="90"/>
+      <c r="A30" s="91" t="s">
+        <v>411</v>
+      </c>
+      <c r="B30" s="91"/>
+      <c r="C30" s="91"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="91"/>
+      <c r="F30" s="91"/>
+      <c r="G30" s="91"/>
+      <c r="H30" s="91"/>
     </row>
   </sheetData>
   <customSheetViews>
@@ -9070,12 +9082,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9095,10 +9107,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -9197,15 +9209,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>394</v>
+        <v>419</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>395</v>
+        <v>420</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>398</v>
+        <v>421</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -9217,28 +9229,26 @@
         <v>173</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>203</v>
-      </c>
+        <v>423</v>
+      </c>
+      <c r="I6" s="3"/>
       <c r="J6" s="3"/>
-      <c r="K6" s="19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>420</v>
+        <v>394</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>421</v>
+        <v>395</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>223</v>
@@ -9247,15 +9257,110 @@
         <v>205</v>
       </c>
       <c r="F7" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
+        <v>322</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>324</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E9" s="83" t="s">
+        <v>205</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>428</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
         <v>1</v>
       </c>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="6" t="s">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="6" t="s">
         <v>162</v>
       </c>
     </row>
@@ -9277,12 +9382,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9302,10 +9407,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="88" t="s">
         <v>402</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="89"/>
     </row>
     <row r="3" spans="1:11" s="13" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="34" t="s">
@@ -9342,7 +9447,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>403</v>
       </c>
@@ -9350,7 +9455,7 @@
         <v>404</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>409</v>
+        <v>426</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -9365,7 +9470,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -9373,15 +9478,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>405</v>
+        <v>425</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>410</v>
+        <v>427</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -9393,11 +9498,9 @@
         <v>173</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>415</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="3" t="s">
         <v>203</v>
       </c>
@@ -9406,15 +9509,15 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>408</v>
+        <v>317</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>407</v>
+        <v>318</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -9426,15 +9529,17 @@
         <v>173</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="I6" s="3"/>
+        <v>409</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>203</v>
+      </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="19" t="s">
-        <v>163</v>
+      <c r="K6" s="6" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9445,7 +9550,7 @@
         <v>160</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>223</v>
@@ -9474,7 +9579,7 @@
         <v>395</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>223</v>
@@ -9503,7 +9608,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>223</v>
@@ -9524,32 +9629,63 @@
         <v>163</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>420</v>
+        <v>322</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="E10" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="C10" s="71" t="s">
+        <v>324</v>
+      </c>
+      <c r="D10" s="72" t="s">
+        <v>223</v>
+      </c>
+      <c r="E10" s="83" t="s">
         <v>205</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="72" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" s="3"/>
+      <c r="K10" s="25" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
+        <v>413</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2">
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
         <v>1</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="6" t="s">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="6" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Arelda Version 4.0 -> 4.1
</commit_message>
<xml_diff>
--- a/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
+++ b/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573" firstSheet="6" activeTab="8"/>
+    <workbookView xWindow="-15" yWindow="5970" windowWidth="25260" windowHeight="6030" tabRatio="573"/>
   </bookViews>
   <sheets>
     <sheet name="Titelblatt" sheetId="1" r:id="rId1"/>
@@ -1076,9 +1076,6 @@
     <t>Über die Gesamtheit der AIP eindeutige ID im Zusammenhang mit Paketmigrationen. Entsteht zum ersten Mal, wenn ein AIP migriert wird.</t>
   </si>
   <si>
-    <t>4.0</t>
-  </si>
-  <si>
     <t>MD5, SHA-1, SHA-256, SHA-512</t>
   </si>
   <si>
@@ -1158,9 +1155,6 @@
   </si>
   <si>
     <t>text (token)</t>
-  </si>
-  <si>
-    <t>März 2012</t>
   </si>
   <si>
     <t>Markierung, die angibt, ob sich in den Dokumenten des Dossiers oder der Unterlagengruppe besonders schützenswerten Personendaten oder Persönlichkeitsprofilen gemäss Datenschutzrecht befinden</t>
@@ -1622,6 +1616,12 @@
   </si>
   <si>
     <t>Geschäftsart - Differenzbereinigung</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>April 2015</t>
   </si>
 </sst>
 </file>
@@ -2301,21 +2301,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2325,16 +2310,31 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3617,8 +3617,8 @@
   </sheetPr>
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3660,7 +3660,7 @@
         <v>229</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>335</v>
+        <v>428</v>
       </c>
       <c r="D7" s="45"/>
       <c r="E7" s="45"/>
@@ -3673,7 +3673,7 @@
         <v>230</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>307</v>
+        <v>427</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
@@ -3790,9 +3790,6 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="18" max="16383" man="1"/>
   </rowBreaks>
-  <ignoredErrors>
-    <ignoredError sqref="C8" numberStoredAsText="1"/>
-  </ignoredErrors>
   <drawing r:id="rId3"/>
 </worksheet>
 </file>
@@ -4326,13 +4323,13 @@
     </row>
     <row r="19" spans="1:11" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D19" s="72" t="s">
         <v>223</v>
@@ -4490,7 +4487,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -4505,7 +4502,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
@@ -4646,7 +4643,7 @@
         <v>167</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -4677,7 +4674,7 @@
         <v>135</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -4749,7 +4746,7 @@
         <v>204</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>40</v>
@@ -5507,7 +5504,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="92" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B1" s="93"/>
       <c r="C1" s="48"/>
@@ -5570,13 +5567,13 @@
     </row>
     <row r="4" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
+        <v>309</v>
+      </c>
+      <c r="B4" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="C4" s="71" t="s">
         <v>311</v>
-      </c>
-      <c r="C4" s="71" t="s">
-        <v>312</v>
       </c>
       <c r="D4" s="74" t="s">
         <v>205</v>
@@ -5591,7 +5588,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="25" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I4" s="72"/>
       <c r="J4" s="72"/>
@@ -5601,13 +5598,13 @@
     </row>
     <row r="5" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
+        <v>313</v>
+      </c>
+      <c r="B5" s="25" t="s">
         <v>314</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="71" t="s">
         <v>315</v>
-      </c>
-      <c r="C5" s="71" t="s">
-        <v>316</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>205</v>
@@ -5630,13 +5627,13 @@
     </row>
     <row r="6" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="71" t="s">
         <v>318</v>
-      </c>
-      <c r="C6" s="71" t="s">
-        <v>319</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>205</v>
@@ -5659,13 +5656,13 @@
     </row>
     <row r="7" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
+        <v>319</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>320</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>321</v>
-      </c>
       <c r="C7" s="69" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>205</v>
@@ -5723,98 +5720,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="54" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="99" t="s">
-        <v>373</v>
-      </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
+      <c r="A1" s="94" t="s">
+        <v>371</v>
+      </c>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
       <c r="D1" s="75"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="95" t="s">
+        <v>368</v>
+      </c>
+      <c r="B4" s="95"/>
+      <c r="C4" s="95"/>
+    </row>
+    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="95" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="100" t="s">
-        <v>370</v>
-      </c>
-      <c r="B4" s="100"/>
-      <c r="C4" s="100"/>
-    </row>
-    <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="100" t="s">
-        <v>371</v>
-      </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="95"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" s="58" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
-        <v>337</v>
-      </c>
-      <c r="B7" s="102" t="s">
-        <v>314</v>
-      </c>
-      <c r="C7" s="103"/>
+        <v>335</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>313</v>
+      </c>
+      <c r="C7" s="100"/>
       <c r="D7" s="77"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="97" t="s">
-        <v>338</v>
-      </c>
-      <c r="C8" s="98"/>
+      <c r="B8" s="101" t="s">
+        <v>336</v>
+      </c>
+      <c r="C8" s="102"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="97" t="s">
-        <v>339</v>
-      </c>
-      <c r="C9" s="98"/>
+      <c r="B9" s="101" t="s">
+        <v>337</v>
+      </c>
+      <c r="C9" s="102"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="97" t="s">
-        <v>340</v>
-      </c>
-      <c r="C10" s="98"/>
+      <c r="B10" s="101" t="s">
+        <v>338</v>
+      </c>
+      <c r="C10" s="102"/>
     </row>
     <row r="11" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="104" t="s">
-        <v>341</v>
-      </c>
-      <c r="C11" s="105"/>
+      <c r="B11" s="103" t="s">
+        <v>339</v>
+      </c>
+      <c r="C11" s="104"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
         <v>218</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="52"/>
       <c r="B13" s="79" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5823,94 +5820,94 @@
         <v>205</v>
       </c>
       <c r="C14" s="56" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="97" t="s">
-        <v>347</v>
-      </c>
-      <c r="C15" s="98"/>
+      <c r="B15" s="101" t="s">
+        <v>345</v>
+      </c>
+      <c r="C15" s="102"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="97" t="s">
-        <v>348</v>
-      </c>
-      <c r="C16" s="98"/>
+      <c r="B16" s="101" t="s">
+        <v>346</v>
+      </c>
+      <c r="C16" s="102"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="97" t="s">
-        <v>349</v>
-      </c>
-      <c r="C17" s="98"/>
+      <c r="B17" s="101" t="s">
+        <v>347</v>
+      </c>
+      <c r="C17" s="102"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
-        <v>350</v>
-      </c>
-      <c r="B18" s="97" t="s">
-        <v>351</v>
-      </c>
-      <c r="C18" s="98"/>
+        <v>348</v>
+      </c>
+      <c r="B18" s="101" t="s">
+        <v>349</v>
+      </c>
+      <c r="C18" s="102"/>
     </row>
     <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="97" t="s">
-        <v>352</v>
-      </c>
-      <c r="C19" s="98"/>
+      <c r="B19" s="101" t="s">
+        <v>350</v>
+      </c>
+      <c r="C19" s="102"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
-        <v>374</v>
-      </c>
-      <c r="B20" s="97" t="s">
-        <v>353</v>
-      </c>
-      <c r="C20" s="98"/>
+        <v>372</v>
+      </c>
+      <c r="B20" s="101" t="s">
+        <v>351</v>
+      </c>
+      <c r="C20" s="102"/>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:4" s="58" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="61" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D22" s="77"/>
     </row>
     <row r="23" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="100" t="s">
-        <v>375</v>
-      </c>
-      <c r="B23" s="101"/>
-      <c r="C23" s="101"/>
+      <c r="A23" s="95" t="s">
+        <v>373</v>
+      </c>
+      <c r="B23" s="96"/>
+      <c r="C23" s="96"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="65" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B25" s="64"/>
       <c r="C25" s="64"/>
     </row>
     <row r="26" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="62" t="s">
+        <v>352</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>353</v>
+      </c>
+      <c r="C26" s="70" t="s">
         <v>354</v>
-      </c>
-      <c r="B26" s="63" t="s">
-        <v>355</v>
-      </c>
-      <c r="C26" s="70" t="s">
-        <v>356</v>
       </c>
       <c r="D26" s="77"/>
     </row>
@@ -5922,7 +5919,7 @@
         <v>15</v>
       </c>
       <c r="C27" s="59" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5933,7 +5930,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="59" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5944,7 +5941,7 @@
         <v>17</v>
       </c>
       <c r="C29" s="59" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5955,7 +5952,7 @@
         <v>18</v>
       </c>
       <c r="C30" s="59" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -5963,140 +5960,151 @@
     </row>
     <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="65" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="C32" s="82"/>
     </row>
     <row r="33" spans="1:4" s="58" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="62" t="s">
+        <v>352</v>
+      </c>
+      <c r="B33" s="63" t="s">
+        <v>353</v>
+      </c>
+      <c r="C33" s="70" t="s">
         <v>354</v>
       </c>
-      <c r="B33" s="63" t="s">
-        <v>355</v>
-      </c>
-      <c r="C33" s="70" t="s">
-        <v>356</v>
-      </c>
       <c r="D33" s="77"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="94" t="s">
+      <c r="A34" s="97" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="94" t="s">
+      <c r="B34" s="97" t="s">
         <v>205</v>
       </c>
       <c r="C34" s="55" t="s">
+        <v>359</v>
+      </c>
+      <c r="D34" s="78"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="98"/>
+      <c r="B35" s="98"/>
+      <c r="C35" s="60" t="s">
+        <v>360</v>
+      </c>
+      <c r="D35" s="78"/>
+    </row>
+    <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="98"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="D36" s="78"/>
+    </row>
+    <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="98"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="66" t="s">
+        <v>377</v>
+      </c>
+      <c r="D37" s="78"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="97" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="97"/>
+      <c r="C38" s="55" t="s">
         <v>361</v>
       </c>
-      <c r="D34" s="78"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="95"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="60" t="s">
+      <c r="D38" s="78"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="98"/>
+      <c r="B39" s="98"/>
+      <c r="C39" s="60" t="s">
         <v>362</v>
       </c>
-      <c r="D35" s="78"/>
-    </row>
-    <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="95"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="60" t="s">
+      <c r="D39" s="78"/>
+    </row>
+    <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="98"/>
+      <c r="B40" s="98"/>
+      <c r="C40" s="60" t="s">
         <v>378</v>
       </c>
-      <c r="D36" s="78"/>
-    </row>
-    <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="95"/>
-      <c r="B37" s="95"/>
-      <c r="C37" s="66" t="s">
+      <c r="D40" s="78"/>
+    </row>
+    <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="98"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="66" t="s">
+        <v>388</v>
+      </c>
+      <c r="D41" s="78"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="97" t="s">
+        <v>363</v>
+      </c>
+      <c r="B42" s="97"/>
+      <c r="C42" s="55" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="A43" s="98"/>
+      <c r="B43" s="98"/>
+      <c r="C43" s="60" t="s">
         <v>379</v>
       </c>
-      <c r="D37" s="78"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="94" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="55" t="s">
-        <v>363</v>
-      </c>
-      <c r="D38" s="78"/>
-    </row>
-    <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="95"/>
-      <c r="B39" s="95"/>
-      <c r="C39" s="60" t="s">
-        <v>364</v>
-      </c>
-      <c r="D39" s="78"/>
-    </row>
-    <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="95"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="60" t="s">
+    </row>
+    <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="98"/>
+      <c r="B44" s="98"/>
+      <c r="C44" s="66" t="s">
         <v>380</v>
       </c>
-      <c r="D40" s="78"/>
-    </row>
-    <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="95"/>
-      <c r="B41" s="95"/>
-      <c r="C41" s="66" t="s">
-        <v>390</v>
-      </c>
-      <c r="D41" s="78"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="94" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="B42" s="94"/>
-      <c r="C42" s="55" t="s">
+      <c r="B45" s="97"/>
+      <c r="C45" s="67" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="95"/>
-      <c r="B43" s="95"/>
-      <c r="C43" s="60" t="s">
+    <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="98"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="60" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="95"/>
-      <c r="B44" s="95"/>
-      <c r="C44" s="66" t="s">
+    <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="105"/>
+      <c r="B47" s="105"/>
+      <c r="C47" s="68" t="s">
         <v>382</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="94" t="s">
-        <v>367</v>
-      </c>
-      <c r="B45" s="94"/>
-      <c r="C45" s="67" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="95"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="60" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="96"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="68" t="s">
-        <v>384</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
@@ -6109,17 +6117,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6356,13 +6353,13 @@
     </row>
     <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>326</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="69" t="s">
         <v>328</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>329</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>205</v>
@@ -6374,10 +6371,10 @@
         <v>173</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H9" s="69" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
@@ -6387,13 +6384,13 @@
     </row>
     <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
+        <v>330</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="23" t="s">
         <v>332</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>333</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>20</v>
@@ -6402,7 +6399,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G10" s="69">
         <v>4</v>
@@ -6418,13 +6415,13 @@
     </row>
     <row r="11" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C11" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D11" s="72" t="s">
         <v>223</v>
@@ -6552,7 +6549,7 @@
         <v>125</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>223</v>
@@ -6836,7 +6833,7 @@
         <v>193</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>223</v>
@@ -6934,13 +6931,13 @@
     </row>
     <row r="15" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C15" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D15" s="72" t="s">
         <v>223</v>
@@ -7639,13 +7636,13 @@
     </row>
     <row r="9" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D9" s="72" t="s">
         <v>223</v>
@@ -8139,13 +8136,13 @@
     </row>
     <row r="16" spans="1:12" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C16" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D16" s="72" t="s">
         <v>223</v>
@@ -8273,7 +8270,7 @@
         <v>156</v>
       </c>
       <c r="C4" s="69" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>20</v>
@@ -8790,7 +8787,7 @@
         <v>104</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>223</v>
@@ -8908,7 +8905,7 @@
     </row>
     <row r="25" spans="1:12" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>186</v>
@@ -9003,13 +9000,13 @@
     </row>
     <row r="28" spans="1:12" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C28" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D28" s="72" t="s">
         <v>223</v>
@@ -9034,7 +9031,7 @@
     </row>
     <row r="30" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="91" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B30" s="91"/>
       <c r="C30" s="91"/>
@@ -9108,7 +9105,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="88" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B1" s="89"/>
     </row>
@@ -9155,7 +9152,7 @@
         <v>157</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -9170,7 +9167,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -9180,13 +9177,13 @@
     </row>
     <row r="5" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -9201,7 +9198,7 @@
         <v>18</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
@@ -9211,13 +9208,13 @@
     </row>
     <row r="6" spans="1:11" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
+        <v>417</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>419</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -9232,7 +9229,7 @@
         <v>17</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -9242,13 +9239,13 @@
     </row>
     <row r="7" spans="1:11" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>223</v>
@@ -9263,7 +9260,7 @@
         <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>203</v>
@@ -9281,7 +9278,7 @@
         <v>159</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>223</v>
@@ -9304,13 +9301,13 @@
     </row>
     <row r="9" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C9" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D9" s="72" t="s">
         <v>223</v>
@@ -9325,7 +9322,7 @@
         <v>18</v>
       </c>
       <c r="H9" s="23" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="I9" s="72" t="s">
         <v>166</v>
@@ -9337,13 +9334,13 @@
     </row>
     <row r="10" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
+        <v>411</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>415</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>223</v>
@@ -9384,10 +9381,10 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9408,7 +9405,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="88" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B1" s="89"/>
     </row>
@@ -9449,13 +9446,13 @@
     </row>
     <row r="4" spans="1:11" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>20</v>
@@ -9470,7 +9467,7 @@
         <v>17</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -9480,13 +9477,13 @@
     </row>
     <row r="5" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>223</v>
@@ -9511,13 +9508,13 @@
     </row>
     <row r="6" spans="1:11" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>318</v>
-      </c>
       <c r="C6" s="2" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>223</v>
@@ -9532,7 +9529,7 @@
         <v>17</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>203</v>
@@ -9550,7 +9547,7 @@
         <v>160</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>223</v>
@@ -9559,7 +9556,7 @@
         <v>205</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -9573,13 +9570,13 @@
     </row>
     <row r="8" spans="1:11" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>223</v>
@@ -9608,7 +9605,7 @@
         <v>159</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>223</v>
@@ -9631,13 +9628,13 @@
     </row>
     <row r="10" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="71" t="s">
         <v>323</v>
-      </c>
-      <c r="C10" s="71" t="s">
-        <v>324</v>
       </c>
       <c r="D10" s="72" t="s">
         <v>223</v>
@@ -9662,13 +9659,13 @@
     </row>
     <row r="11" spans="1:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>414</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>223</v>

</xml_diff>

<commit_message>
Letzte Änderungswünsche aus der Vernehmlassung bis 1.4.2015
</commit_message>
<xml_diff>
--- a/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
+++ b/STAN_d_DRA_2014-xx-xx_eCH-0160_V1.1_ArchivischeAblieferungsschnittstelle_DataDictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\eCH\Fachgruppe_Digitale_Archivierung\eCH-0160\v1.1\05_Entwurf_v1.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\KOST\Standards\eCH\eCH-0160\v1.1\0_Entwurf\05_Entwurf_v1.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="430">
   <si>
     <t xml:space="preserve">Systeme, die mit dem beschriebenen System Daten ausgetauscht haben und damit Subsysteme, Parallelsysteme oder übergeordnete Systeme sind. Hier werden die Bezeichnungen der Systeme und die Art der Verwandtschaft eingetragen. </t>
   </si>
@@ -1622,6 +1622,9 @@
   </si>
   <si>
     <t>April 2015</t>
+  </si>
+  <si>
+    <t>4.0, 4.1</t>
   </si>
 </sst>
 </file>
@@ -2301,6 +2304,21 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2310,31 +2328,16 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3618,7 +3621,7 @@
   <dimension ref="A1:M57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5720,11 +5723,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="54" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="99" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
       <c r="D1" s="75"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5734,65 +5737,65 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="95" t="s">
+      <c r="A4" s="100" t="s">
         <v>368</v>
       </c>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
     </row>
     <row r="5" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="95" t="s">
+      <c r="A5" s="100" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:4" s="58" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>335</v>
       </c>
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="102" t="s">
         <v>313</v>
       </c>
-      <c r="C7" s="100"/>
+      <c r="C7" s="103"/>
       <c r="D7" s="77"/>
     </row>
     <row r="8" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="97" t="s">
         <v>336</v>
       </c>
-      <c r="C8" s="102"/>
+      <c r="C8" s="98"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="50" t="s">
         <v>216</v>
       </c>
-      <c r="B9" s="101" t="s">
+      <c r="B9" s="97" t="s">
         <v>337</v>
       </c>
-      <c r="C9" s="102"/>
+      <c r="C9" s="98"/>
     </row>
     <row r="10" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="97" t="s">
         <v>338</v>
       </c>
-      <c r="C10" s="102"/>
+      <c r="C10" s="98"/>
     </row>
     <row r="11" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
         <v>217</v>
       </c>
-      <c r="B11" s="103" t="s">
+      <c r="B11" s="104" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="104"/>
+      <c r="C11" s="105"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
@@ -5827,55 +5830,55 @@
       <c r="A15" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B15" s="101" t="s">
+      <c r="B15" s="97" t="s">
         <v>345</v>
       </c>
-      <c r="C15" s="102"/>
+      <c r="C15" s="98"/>
     </row>
     <row r="16" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="50" t="s">
         <v>220</v>
       </c>
-      <c r="B16" s="101" t="s">
+      <c r="B16" s="97" t="s">
         <v>346</v>
       </c>
-      <c r="C16" s="102"/>
+      <c r="C16" s="98"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="97" t="s">
         <v>347</v>
       </c>
-      <c r="C17" s="102"/>
+      <c r="C17" s="98"/>
     </row>
     <row r="18" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="57" t="s">
         <v>348</v>
       </c>
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="97" t="s">
         <v>349</v>
       </c>
-      <c r="C18" s="102"/>
+      <c r="C18" s="98"/>
     </row>
     <row r="19" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="50" t="s">
         <v>222</v>
       </c>
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="97" t="s">
         <v>350</v>
       </c>
-      <c r="C19" s="102"/>
+      <c r="C19" s="98"/>
     </row>
     <row r="20" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="50" t="s">
         <v>372</v>
       </c>
-      <c r="B20" s="101" t="s">
+      <c r="B20" s="97" t="s">
         <v>351</v>
       </c>
-      <c r="C20" s="102"/>
+      <c r="C20" s="98"/>
     </row>
     <row r="21" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:4" s="58" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -5885,11 +5888,11 @@
       <c r="D22" s="77"/>
     </row>
     <row r="23" spans="1:4" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="s">
+      <c r="A23" s="100" t="s">
         <v>373</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
+      <c r="B23" s="101"/>
+      <c r="C23" s="101"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
@@ -5977,10 +5980,10 @@
       <c r="D33" s="77"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="97" t="s">
+      <c r="A34" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="B34" s="97" t="s">
+      <c r="B34" s="94" t="s">
         <v>205</v>
       </c>
       <c r="C34" s="55" t="s">
@@ -5989,122 +5992,111 @@
       <c r="D34" s="78"/>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="98"/>
-      <c r="B35" s="98"/>
+      <c r="A35" s="95"/>
+      <c r="B35" s="95"/>
       <c r="C35" s="60" t="s">
         <v>360</v>
       </c>
       <c r="D35" s="78"/>
     </row>
     <row r="36" spans="1:4" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="98"/>
-      <c r="B36" s="98"/>
+      <c r="A36" s="95"/>
+      <c r="B36" s="95"/>
       <c r="C36" s="60" t="s">
         <v>376</v>
       </c>
       <c r="D36" s="78"/>
     </row>
     <row r="37" spans="1:4" ht="79.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="98"/>
-      <c r="B37" s="98"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="66" t="s">
         <v>377</v>
       </c>
       <c r="D37" s="78"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="97"/>
+      <c r="B38" s="94"/>
       <c r="C38" s="55" t="s">
         <v>361</v>
       </c>
       <c r="D38" s="78"/>
     </row>
     <row r="39" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="98"/>
-      <c r="B39" s="98"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="95"/>
       <c r="C39" s="60" t="s">
         <v>362</v>
       </c>
       <c r="D39" s="78"/>
     </row>
     <row r="40" spans="1:4" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="98"/>
-      <c r="B40" s="98"/>
+      <c r="A40" s="95"/>
+      <c r="B40" s="95"/>
       <c r="C40" s="60" t="s">
         <v>378</v>
       </c>
       <c r="D40" s="78"/>
     </row>
     <row r="41" spans="1:4" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="98"/>
-      <c r="B41" s="98"/>
+      <c r="A41" s="95"/>
+      <c r="B41" s="95"/>
       <c r="C41" s="66" t="s">
         <v>388</v>
       </c>
       <c r="D41" s="78"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="97" t="s">
+      <c r="A42" s="94" t="s">
         <v>363</v>
       </c>
-      <c r="B42" s="97"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="55" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="51" x14ac:dyDescent="0.2">
-      <c r="A43" s="98"/>
-      <c r="B43" s="98"/>
+      <c r="A43" s="95"/>
+      <c r="B43" s="95"/>
       <c r="C43" s="60" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="98"/>
-      <c r="B44" s="98"/>
+      <c r="A44" s="95"/>
+      <c r="B44" s="95"/>
       <c r="C44" s="66" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="97" t="s">
+      <c r="A45" s="94" t="s">
         <v>365</v>
       </c>
-      <c r="B45" s="97"/>
+      <c r="B45" s="94"/>
       <c r="C45" s="67" t="s">
         <v>366</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="98"/>
-      <c r="B46" s="98"/>
+      <c r="A46" s="95"/>
+      <c r="B46" s="95"/>
       <c r="C46" s="60" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="105"/>
-      <c r="B47" s="105"/>
+      <c r="A47" s="96"/>
+      <c r="B47" s="96"/>
       <c r="C47" s="68" t="s">
         <v>382</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A42:A44"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="B34:B37"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
@@ -6117,6 +6109,17 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B15:C15"/>
+    <mergeCell ref="A42:A44"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="B34:B37"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6137,7 +6140,7 @@
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F34" sqref="F34"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6401,11 +6404,11 @@
       <c r="F10" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="G10" s="69">
-        <v>4</v>
+      <c r="G10" s="69" t="s">
+        <v>429</v>
       </c>
       <c r="H10" s="23">
-        <v>4</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>

</xml_diff>